<commit_message>
Signed-off-by: Krishna Patel <kishupatel694@gmail.com>
</commit_message>
<xml_diff>
--- a/Assignment/Module 2/Assignment 2 Testcases.xlsx
+++ b/Assignment/Module 2/Assignment 2 Testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23aa3cb755853b5b/Desktop/Tops/Assignment/Module 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="342" documentId="11_F25DC773A252ABDACC104856611978385ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B315F52-1307-49A5-9060-38E1FC768693}"/>
+  <xr:revisionPtr revIDLastSave="344" documentId="11_F25DC773A252ABDACC104856611978385ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADF75282-32A5-4D64-B050-9B5082F20DD2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HLR-INSTA" sheetId="1" r:id="rId1"/>
@@ -1690,16 +1690,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1722,11 +1716,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1741,6 +1731,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2041,13 +2037,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2062,7 +2058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.5">
+    <row r="3" spans="1:3" ht="29">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2073,7 +2069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="58">
+    <row r="4" spans="1:3" ht="43.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2084,7 +2080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="58">
+    <row r="5" spans="1:3" ht="43.5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2182,11 +2178,11 @@
       <c r="C15" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="30" customHeight="1">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:4" ht="29">
       <c r="A18" s="1">
@@ -2367,765 +2363,765 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="29">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.5">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="58">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="43.5">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="29">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="29">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="29">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="29">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="29">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>1</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="H11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>2</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="43.5">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="29">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>2</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="6" t="s">
+      <c r="H16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="29">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>14</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>2</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="29">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>2</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="H18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="29">
-      <c r="A19" s="6">
+      <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>2</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="6" t="s">
+      <c r="H19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="29">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>2</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="6" t="s">
+      <c r="H20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="29">
-      <c r="A21" s="6">
+      <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <v>2</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" s="6" t="s">
+      <c r="H21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="6">
+      <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <v>2</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="6" t="s">
+      <c r="H22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="29">
-      <c r="A23" s="6">
+      <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <v>2</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I23" s="6" t="s">
+      <c r="H23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="29">
-      <c r="A24" s="6">
+      <c r="A24" s="4">
         <v>21</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="4">
         <v>2</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I24" s="6" t="s">
+      <c r="H24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="6">
+      <c r="A25" s="4">
         <v>22</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="4">
         <v>2</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I25" s="6" t="s">
+      <c r="H25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="29">
-      <c r="A26" s="6">
+      <c r="A26" s="4">
         <v>23</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="4">
         <v>2</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I26" s="6" t="s">
+      <c r="H26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="29">
-      <c r="A27" s="6">
+      <c r="A27" s="4">
         <v>24</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="4">
         <v>2</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" s="6" t="s">
+      <c r="H27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="6">
+      <c r="A28" s="4">
         <v>25</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="4">
         <v>2</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I28" s="6" t="s">
+      <c r="H28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3142,7 +3138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCA59DA-F3CB-4893-A8B1-33D7E034BDB3}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -3154,13 +3150,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
@@ -3372,8 +3368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42015562-431B-44AC-B24E-E4CFC279DBCC}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3388,35 +3384,35 @@
     <col min="9" max="9" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="29">
       <c r="A2" s="1">
@@ -3434,7 +3430,7 @@
       <c r="E2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -3550,7 +3546,7 @@
       <c r="E6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>71</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -3912,9 +3908,7 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -3925,9 +3919,7 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -4106,68 +4098,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.5" customHeight="1">
-      <c r="A2" s="11">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="1" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="31.5" customHeight="1">
-      <c r="A3" s="11">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="1" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.5" customHeight="1">
-      <c r="A4" s="11">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" t="s">
         <v>243</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="1" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28" customHeight="1">
-      <c r="A5" s="11">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" t="s">
         <v>245</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="1" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" customHeight="1">
-      <c r="A6" s="11">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="1" t="s">
         <v>248</v>
       </c>
     </row>
@@ -4197,321 +4189,321 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="42.5">
-      <c r="A2" s="14">
+    <row r="2" spans="1:9" ht="28.5">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="10">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="42.5">
-      <c r="A3" s="14">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="56.5">
-      <c r="A4" s="14">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>3</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.5">
-      <c r="A5" s="14">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>3.1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="42.5">
-      <c r="A6" s="14">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="10">
         <v>3.2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.5">
-      <c r="A7" s="14">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="10">
         <v>3.3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="42.5">
-      <c r="A8" s="14">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="10">
         <v>4</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="42.5">
-      <c r="A9" s="14">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="42.5">
-      <c r="A10" s="14">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="10">
         <v>4.2</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.5">
-      <c r="A11" s="14">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="10" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4539,409 +4531,409 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="29">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="29">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="29">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="6">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="6">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="6">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="6">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="6">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="6">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="6">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="6">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="6">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="6">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="6">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="6">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="6">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="6">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="4" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="6">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="4" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="6">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="4" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="6">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="4" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="6">
+      <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>351</v>
       </c>
     </row>
@@ -4969,1016 +4961,1016 @@
     <col min="8" max="8" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="29">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="29">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>9</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>10</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>11</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="H11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>12</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="6" t="s">
+      <c r="H12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>13</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="H13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>14</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>15</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>16</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="6" t="s">
+      <c r="H16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>17</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="29">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>18</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="H18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="6">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>19</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="6" t="s">
+      <c r="H19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>20</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="6" t="s">
+      <c r="H20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="6">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <v>21</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" s="6" t="s">
+      <c r="H21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="29">
-      <c r="A22" s="6">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <v>22</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="6" t="s">
+      <c r="H22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="6">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <v>23</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I23" s="6" t="s">
+      <c r="H23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="6">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="4">
         <v>24</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I24" s="6" t="s">
+      <c r="H24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="6">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="4">
         <v>25</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I25" s="6" t="s">
+      <c r="H25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="6">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="4">
         <v>26</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I26" s="6" t="s">
+      <c r="H26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="6">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="4">
         <v>27</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" s="6" t="s">
+      <c r="H27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="6">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="4">
         <v>28</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I28" s="6" t="s">
+      <c r="H28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="6">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="4">
         <v>29</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I29" s="6" t="s">
+      <c r="H29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="6">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="4">
         <v>30</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I30" s="6" t="s">
+      <c r="H30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I30" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="6">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="4">
         <v>31</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I31" s="6" t="s">
+      <c r="H31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="6">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="4">
         <v>32</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I32" s="6" t="s">
+      <c r="H32" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I32" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="6">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="4">
         <v>33</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G33" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I33" s="6" t="s">
+      <c r="H33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="6">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="4">
         <v>34</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I34" s="6" t="s">
+      <c r="H34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="6">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="4">
         <v>36</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="G35" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I35" s="6" t="s">
+      <c r="H35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I35" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -6011,611 +6003,611 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="43.5">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="58">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="58">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="43.5">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>3.1</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="29">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="29">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="29">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="29">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="29">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="H11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="29">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="6" t="s">
+      <c r="H12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="29">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="H13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="29">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>11</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="29">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>12</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="29">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>13</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="6" t="s">
+      <c r="H16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="29">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>14</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="29">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>15</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="H18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="29">
-      <c r="A19" s="6">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>16</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="6" t="s">
+      <c r="H19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="29">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>17</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="6" t="s">
+      <c r="H20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="29">
-      <c r="A21" s="6">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <v>18</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" s="6" t="s">
+      <c r="H21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>